<commit_message>
first MM models, mistakes visualization corrected
</commit_message>
<xml_diff>
--- a/data/results/00_inferentialResults.xlsx
+++ b/data/results/00_inferentialResults.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga84kuj\Documents\R\Multilab_Analysis\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DC05D2-BA32-414E-ADFB-E837689A261A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A106425D-B156-455A-8EDA-666119B2660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ANOVA_UsabQ" sheetId="2" r:id="rId1"/>
     <sheet name="CLM_UsabQ" sheetId="3" r:id="rId2"/>
     <sheet name="TOST_UsabQ" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TOST_UsabQ!$A$1:$AM$25</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -696,7 +699,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,6 +718,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -728,15 +737,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3623,8 +3643,8 @@
   <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q24" sqref="Q24"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3634,7 +3654,7 @@
     <col min="3" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="11" width="12.7109375" customWidth="1"/>
+    <col min="9" max="11" width="12.7109375" hidden="1" customWidth="1"/>
     <col min="12" max="14" width="13.42578125" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" customWidth="1"/>
@@ -4527,83 +4547,83 @@
         <v>0.38231295667591675</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
-      <c r="A12" t="s">
+    <row r="12" spans="1:26" s="3" customFormat="1">
+      <c r="A12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>0.44173546981448902</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>0.14970960071335301</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>0.17259227417182499</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>0.25009585933650502</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>0.248032174848586</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <v>0.34843930570681803</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>1.7662646274368401</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="3">
         <v>0.60358943675249099</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="3">
         <v>0.49532952036429201</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="3">
         <v>7.73514630534924E-2</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>0.54611663747820804</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="3">
         <v>0.62036753621135499</v>
       </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="S12">
-        <v>1</v>
-      </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12">
+      <c r="R12" s="3">
+        <v>1</v>
+      </c>
+      <c r="S12" s="3">
+        <v>1</v>
+      </c>
+      <c r="T12" s="3">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
         <v>0.73826674694419925</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="3">
         <v>7.1094532540249677E-3</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="3">
         <v>0.24535133374431928</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="3">
         <v>0.39021666716514758</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="3">
         <v>0.93280394027316826</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="3">
         <v>0.62036753621135488</v>
       </c>
     </row>
@@ -5329,7 +5349,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="X1:Z1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5339,10 +5359,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" activeCellId="5" sqref="A20:XFD20 A18:XFD18 A16:XFD16 A14:XFD14 A12:XFD12 A10:XFD10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5374,8 +5395,8 @@
     <col min="27" max="27" width="14.7109375" customWidth="1"/>
     <col min="28" max="28" width="15.5703125" customWidth="1"/>
     <col min="29" max="29" width="15.7109375" customWidth="1"/>
-    <col min="30" max="30" width="18.7109375" customWidth="1"/>
-    <col min="31" max="31" width="18.85546875" customWidth="1"/>
+    <col min="30" max="30" width="18.7109375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="18.85546875" style="1" customWidth="1"/>
     <col min="32" max="32" width="15.5703125" customWidth="1"/>
     <col min="33" max="33" width="18" customWidth="1"/>
     <col min="34" max="34" width="18.140625" customWidth="1"/>
@@ -5474,10 +5495,10 @@
       <c r="AC1" t="s">
         <v>186</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>188</v>
       </c>
       <c r="AF1" t="s">
@@ -5505,7 +5526,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" hidden="1">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -5624,7 +5645,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" hidden="1">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -5743,7 +5764,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" hidden="1">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -5862,7 +5883,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" hidden="1">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -5981,7 +6002,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" hidden="1">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -6100,7 +6121,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" hidden="1">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -6219,7 +6240,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" hidden="1">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -6338,7 +6359,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" hidden="1">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -6457,7 +6478,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" hidden="1">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -6576,7 +6597,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" hidden="1">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -6664,10 +6685,10 @@
       <c r="AC11">
         <v>1201.5</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="1">
         <v>1555</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="1">
         <v>864</v>
       </c>
       <c r="AF11">
@@ -6695,7 +6716,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" hidden="1">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -6814,7 +6835,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" hidden="1">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -6902,10 +6923,10 @@
       <c r="AC13">
         <v>983</v>
       </c>
-      <c r="AD13">
+      <c r="AD13" s="1">
         <v>1440</v>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="1">
         <v>521</v>
       </c>
       <c r="AF13">
@@ -6933,7 +6954,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" hidden="1">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -7052,7 +7073,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" hidden="1">
       <c r="A15" t="s">
         <v>148</v>
       </c>
@@ -7140,10 +7161,10 @@
       <c r="AC15">
         <v>1026.5</v>
       </c>
-      <c r="AD15">
+      <c r="AD15" s="1">
         <v>1396</v>
       </c>
-      <c r="AE15">
+      <c r="AE15" s="1">
         <v>691</v>
       </c>
       <c r="AF15">
@@ -7171,7 +7192,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" hidden="1">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -7290,7 +7311,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" hidden="1">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -7378,10 +7399,10 @@
       <c r="AC17">
         <v>1160</v>
       </c>
-      <c r="AD17">
+      <c r="AD17" s="1">
         <v>1628</v>
       </c>
-      <c r="AE17">
+      <c r="AE17" s="1">
         <v>750</v>
       </c>
       <c r="AF17">
@@ -7409,7 +7430,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" hidden="1">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -7528,7 +7549,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" hidden="1">
       <c r="A19" t="s">
         <v>152</v>
       </c>
@@ -7616,10 +7637,10 @@
       <c r="AC19">
         <v>1048.5</v>
       </c>
-      <c r="AD19">
+      <c r="AD19" s="1">
         <v>1414</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="1">
         <v>667</v>
       </c>
       <c r="AF19">
@@ -7647,7 +7668,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" hidden="1">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -7766,7 +7787,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" hidden="1">
       <c r="A21" t="s">
         <v>154</v>
       </c>
@@ -7854,10 +7875,10 @@
       <c r="AC21">
         <v>1090</v>
       </c>
-      <c r="AD21">
+      <c r="AD21" s="1">
         <v>1424</v>
       </c>
-      <c r="AE21">
+      <c r="AE21" s="1">
         <v>805</v>
       </c>
       <c r="AF21">
@@ -8123,7 +8144,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" hidden="1">
       <c r="A24" t="s">
         <v>157</v>
       </c>
@@ -8242,7 +8263,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" hidden="1">
       <c r="A25" t="s">
         <v>158</v>
       </c>
@@ -8362,8 +8383,16 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F1048576 D1:D1048576 R1:R1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  <autoFilter ref="A1:AM25" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Uebel_12"/>
+        <filter val="Uebel_23"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="F1:F1048576 D1:D1048576 R1:R1048576 AF1:AH1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>